<commit_message>
mise à jour diagramme
</commit_message>
<xml_diff>
--- a/divers/fiche investigation.xlsx
+++ b/divers/fiche investigation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/794ecb4e77428459/Documents/formationDevWeb/Projets/projet7/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="176" documentId="11_AD4D9D64A577C15A4A54184CC09947E05BDEDD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2EE447D6-6BAC-4E4A-AEB6-F6F84B7332D1}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="11_AD4D9D64A577C15A4A54184CC09947E05BDEDD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD35170-1741-4507-9417-2DF4C15E1DB4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Fiche d’investigation de fonctionnalité</t>
   </si>
   <si>
-    <t>Avantages</t>
-  </si>
-  <si>
-    <t>Inconvénients</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fonctionnalité :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : Barre de recherche</t>
+    </r>
   </si>
   <si>
     <r>
@@ -57,7 +74,274 @@
       </rPr>
       <t xml:space="preserve">
 Dans cette option, nous utiliserons principalement des boucles pour rechercher les données des recettes
-dans le fichier Json</t>
+dans la liste des recettes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problématique : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Identifier l'algorithme ayant les meilleurs performances pour accéder rapidement à une recette correspondant depuis la barre de recherche dans la liste des recettes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Avantages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-Syntaxe concise : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La boucle forEach offre une syntaxe plus concise, ce qui rend le code plus lisible.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-Moins de risques d'erreur d'index :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Étant donné que la boucle forEach gère automatiquement l'index, il y a moins de risques d'erreur d'index.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inconvénients</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Manque de contrôle :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vous n'avez pas autant de contrôle sur l'index de la boucle, ce qui peut être un inconvénient dans certaines situations.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Manque de contrôle : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vous n'avez pas autant de contrôle sur l'index de la boucle, ce qui peut être un inconvénient dans certaines situations.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Avantages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+Contrôle total : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La boucle for offre un contrôle total sur l'index de la boucle, ce qui peut être utile dans certaines situations.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Possibilité de sauter des éléments :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vous pouvez utiliser continue pour sauter des éléments qui ne correspondent pas à votre critère de recherche.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Inconvénients
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Syntaxe plus verbeuse :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La syntaxe de la boucle for est généralement plus verbeuse, ce qui peut rendre le code moins lisible.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Risque d'erreur d'index :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> En raison de la manipulation manuelle de l'index, il existe un risque accru d'erreur d'index.</t>
     </r>
   </si>
   <si>
@@ -81,79 +365,37 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-Dans cette option, nous utiliserons principalement les méthode de l'objet array pour rechercher les données des recettes dans le fichier Json</t>
-    </r>
-  </si>
-  <si>
-    <t>Solution retenue :</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Fonctionnalité :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : Filtrer les recettes dans l’interface utilisateur</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Problématique : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Identifier l'algorithme ayant les meilleurs performances pour accéder rapidement à une recette correspondant à un besoin de l’utilisateur dans les recettes déjà reçues</t>
-    </r>
-  </si>
-  <si>
-    <t>Recherche des recettes correspondantes dans TITRE, INGREDIENTS, DESCRIPTION</t>
-  </si>
-  <si>
-    <t>L'utilisateur entre au minimum 3 caractères</t>
-  </si>
-  <si>
-    <t>Actualisé l'interface avec les résultats trouvés</t>
-  </si>
-  <si>
-    <t>Avec des Boucles</t>
-  </si>
-  <si>
-    <t>Utilisateur entre un caractère</t>
+Dans cette option, nous utiliserons principalement la méthode de l'objet array foreach pour rechercher les données des recettes dans la liste des recettes</t>
+    </r>
+  </si>
+  <si>
+    <t>Code plus court et plus lisible, moins de risques d'erreurs</t>
+  </si>
+  <si>
+    <t>Permet de controler l'index et de sauter des éléments</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Solution retenue :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La solution retenue est l'option 2 avec l'utilisation de méthodes d'objets, ici la méthode foreach pour avoir une syntaxe plus concose et un code plus lisible.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,6 +413,15 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -251,23 +502,26 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -278,11 +532,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -617,221 +868,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:J34"/>
+  <dimension ref="A5:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
     </row>
     <row r="6" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
     </row>
     <row r="7" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="10"/>
+    </row>
+    <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="11" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+    </row>
+    <row r="12" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10" t="s">
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="11" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-    </row>
-    <row r="12" spans="1:10" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="A13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
     </row>
     <row r="15" spans="1:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="16" spans="1:10" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
     </row>
     <row r="19" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="A19" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
     </row>
     <row r="23" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C34" t="s">
-        <v>12</v>
-      </c>
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="A17:J17"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="A13:J13"/>
@@ -839,11 +1068,6 @@
     <mergeCell ref="A8:J9"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Mise en place du responsive
</commit_message>
<xml_diff>
--- a/divers/fiche investigation.xlsx
+++ b/divers/fiche investigation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/794ecb4e77428459/Documents/formationDevWeb/Projets/projet7/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="11_AD4D9D64A577C15A4A54184CC09947E05BDEDD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD35170-1741-4507-9417-2DF4C15E1DB4}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="11_AD4D9D64A577C15A4A54184CC09947E05BDEDD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D36FE4B-D059-41FB-B79D-C6C0619CD3C5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Fiche d’investigation de fonctionnalité</t>
   </si>
@@ -81,23 +81,58 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Problématique : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Identifier l'algorithme ayant les meilleurs performances pour accéder rapidement à une recette correspondant depuis la barre de recherche dans la liste des recettes</t>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Avantages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-Syntaxe concise : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La boucle forEach offre une syntaxe plus concise, ce qui rend le code plus lisible.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-Moins de risques d'erreur d'index :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Étant donné que la boucle forEach gère automatiquement l'index, il y a moins de risques d'erreur d'index.</t>
     </r>
   </si>
   <si>
@@ -122,40 +157,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">:
+Contrôle total : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La boucle for offre un contrôle total sur l'index de la boucle, ce qui peut être utile dans certaines situations.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">
--Syntaxe concise : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La boucle forEach offre une syntaxe plus concise, ce qui rend le code plus lisible.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--Moins de risques d'erreur d'index :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Étant donné que la boucle forEach gère automatiquement l'index, il y a moins de risques d'erreur d'index.</t>
+Possibilité de sauter des éléments :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vous pouvez utiliser continue pour sauter des éléments qui ne correspondent pas à votre critère de recherche.</t>
     </r>
   </si>
   <si>
@@ -169,6 +204,100 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">Inconvénients
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Syntaxe plus verbeuse :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La syntaxe de la boucle for est généralement plus verbeuse, ce qui peut rendre le code moins lisible.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Risque d'erreur d'index :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> En raison de la manipulation manuelle de l'index, il existe un risque accru d'erreur d'index.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Option 2 : Recherche les méthodes d'objets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Dans cette option, nous utiliserons principalement la méthode de l'objet array foreach pour rechercher les données des recettes dans la liste des recettes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Inconvénients</t>
     </r>
     <r>
@@ -193,201 +322,44 @@
       </rPr>
       <t xml:space="preserve"> Vous n'avez pas autant de contrôle sur l'index de la boucle, ce qui peut être un inconvénient dans certaines situations.</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Manque de contrôle : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vous n'avez pas autant de contrôle sur l'index de la boucle, ce qui peut être un inconvénient dans certaines situations.</t>
-    </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Avantages</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:
-Contrôle total : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La boucle for offre un contrôle total sur l'index de la boucle, ce qui peut être utile dans certaines situations.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Possibilité de sauter des éléments :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Vous pouvez utiliser continue pour sauter des éléments qui ne correspondent pas à votre critère de recherche.</t>
+      <t xml:space="preserve">Solution retenue :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La solution retenue est l'option 2 avec l'utilisation de méthodes d'objets, cette solution est plus performante, permet d'avoir une syntaxe plus concise, un code plus lisible et moins de risques d'erreurs.</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Inconvénients
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Syntaxe plus verbeuse :</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La syntaxe de la boucle for est généralement plus verbeuse, ce qui peut rendre le code moins lisible.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Risque d'erreur d'index :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> En raison de la manipulation manuelle de l'index, il existe un risque accru d'erreur d'index.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Option 2 : Recherche les méthodes d'objets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Dans cette option, nous utiliserons principalement la méthode de l'objet array foreach pour rechercher les données des recettes dans la liste des recettes</t>
-    </r>
-  </si>
-  <si>
-    <t>Code plus court et plus lisible, moins de risques d'erreurs</t>
-  </si>
-  <si>
-    <t>Permet de controler l'index et de sauter des éléments</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Solution retenue :
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La solution retenue est l'option 2 avec l'utilisation de méthodes d'objets, ici la méthode foreach pour avoir une syntaxe plus concose et un code plus lisible.</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problématique : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Identifier l'algorithme ayant les meilleurs performances pour accéder rapidement à une recette correspondant depuis la barre de recherche.</t>
     </r>
   </si>
 </sst>
@@ -506,6 +478,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -517,12 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -531,9 +506,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,10 +571,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -870,179 +838,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="11" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="15" spans="1:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="19" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="23" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
@@ -1056,11 +1020,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="A17:J17"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="A13:J13"/>
@@ -1068,6 +1027,11 @@
     <mergeCell ref="A8:J9"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix bug mineurs et responsive
</commit_message>
<xml_diff>
--- a/divers/fiche investigation.xlsx
+++ b/divers/fiche investigation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/794ecb4e77428459/Documents/formationDevWeb/Projets/projet7/divers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="221" documentId="11_AD4D9D64A577C15A4A54184CC09947E05BDEDD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4AD35170-1741-4507-9417-2DF4C15E1DB4}"/>
+  <xr:revisionPtr revIDLastSave="227" documentId="11_AD4D9D64A577C15A4A54184CC09947E05BDEDD82" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D36FE4B-D059-41FB-B79D-C6C0619CD3C5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Fiche d’investigation de fonctionnalité</t>
   </si>
@@ -81,23 +81,58 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Problématique : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Identifier l'algorithme ayant les meilleurs performances pour accéder rapidement à une recette correspondant depuis la barre de recherche dans la liste des recettes</t>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Avantages</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-Syntaxe concise : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La boucle forEach offre une syntaxe plus concise, ce qui rend le code plus lisible.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+-Moins de risques d'erreur d'index :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Étant donné que la boucle forEach gère automatiquement l'index, il y a moins de risques d'erreur d'index.</t>
     </r>
   </si>
   <si>
@@ -122,40 +157,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">:
+Contrôle total : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La boucle for offre un contrôle total sur l'index de la boucle, ce qui peut être utile dans certaines situations.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">
--Syntaxe concise : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La boucle forEach offre une syntaxe plus concise, ce qui rend le code plus lisible.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
--Moins de risques d'erreur d'index :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Étant donné que la boucle forEach gère automatiquement l'index, il y a moins de risques d'erreur d'index.</t>
+Possibilité de sauter des éléments :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vous pouvez utiliser continue pour sauter des éléments qui ne correspondent pas à votre critère de recherche.</t>
     </r>
   </si>
   <si>
@@ -169,6 +204,100 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
+      <t xml:space="preserve">Inconvénients
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Syntaxe plus verbeuse :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La syntaxe de la boucle for est généralement plus verbeuse, ce qui peut rendre le code moins lisible.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Risque d'erreur d'index :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> En raison de la manipulation manuelle de l'index, il existe un risque accru d'erreur d'index.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Option 2 : Recherche les méthodes d'objets</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Dans cette option, nous utiliserons principalement la méthode de l'objet array foreach pour rechercher les données des recettes dans la liste des recettes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Inconvénients</t>
     </r>
     <r>
@@ -193,201 +322,44 @@
       </rPr>
       <t xml:space="preserve"> Vous n'avez pas autant de contrôle sur l'index de la boucle, ce qui peut être un inconvénient dans certaines situations.</t>
     </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Manque de contrôle : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Vous n'avez pas autant de contrôle sur l'index de la boucle, ce qui peut être un inconvénient dans certaines situations.</t>
-    </r>
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Avantages</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:
-Contrôle total : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La boucle for offre un contrôle total sur l'index de la boucle, ce qui peut être utile dans certaines situations.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Possibilité de sauter des éléments :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Vous pouvez utiliser continue pour sauter des éléments qui ne correspondent pas à votre critère de recherche.</t>
+      <t xml:space="preserve">Solution retenue :
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>La solution retenue est l'option 2 avec l'utilisation de méthodes d'objets, cette solution est plus performante, permet d'avoir une syntaxe plus concise, un code plus lisible et moins de risques d'erreurs.</t>
     </r>
   </si>
   <si>
     <r>
       <rPr>
         <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Inconvénients
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Syntaxe plus verbeuse :</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La syntaxe de la boucle for est généralement plus verbeuse, ce qui peut rendre le code moins lisible.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Risque d'erreur d'index :</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> En raison de la manipulation manuelle de l'index, il existe un risque accru d'erreur d'index.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Option 2 : Recherche les méthodes d'objets</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Dans cette option, nous utiliserons principalement la méthode de l'objet array foreach pour rechercher les données des recettes dans la liste des recettes</t>
-    </r>
-  </si>
-  <si>
-    <t>Code plus court et plus lisible, moins de risques d'erreurs</t>
-  </si>
-  <si>
-    <t>Permet de controler l'index et de sauter des éléments</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Solution retenue :
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>La solution retenue est l'option 2 avec l'utilisation de méthodes d'objets, ici la méthode foreach pour avoir une syntaxe plus concose et un code plus lisible.</t>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Problématique : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Identifier l'algorithme ayant les meilleurs performances pour accéder rapidement à une recette correspondant depuis la barre de recherche.</t>
     </r>
   </si>
 </sst>
@@ -506,6 +478,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -517,12 +498,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -531,9 +506,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,10 +571,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -870,179 +838,175 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" ht="12.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="9"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
     </row>
     <row r="8" spans="1:10" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="11" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="15" spans="1:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:10" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="11" spans="1:10" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" ht="108.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="11" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" ht="57" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
-    </row>
-    <row r="15" spans="1:10" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="19" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-    </row>
-    <row r="17" spans="1:10" ht="65.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-    </row>
-    <row r="19" spans="1:10" ht="58.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="23" spans="1:10" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
@@ -1056,11 +1020,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A19:J19"/>
-    <mergeCell ref="A15:J15"/>
-    <mergeCell ref="A16:E16"/>
-    <mergeCell ref="F16:J16"/>
-    <mergeCell ref="A17:J17"/>
     <mergeCell ref="A12:E12"/>
     <mergeCell ref="F12:J12"/>
     <mergeCell ref="A13:J13"/>
@@ -1068,6 +1027,11 @@
     <mergeCell ref="A8:J9"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A19:J19"/>
+    <mergeCell ref="A15:J15"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="F16:J16"/>
+    <mergeCell ref="A17:J17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>